<commit_message>
Travail Métro BDD et Interface
</commit_message>
<xml_diff>
--- a/MetroParis.xlsx
+++ b/MetroParis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxia\Documents\Ecole\projet info\Liv-In-Paris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2eef7a2f02062645/Bureau/Programme/S4/Projet Pb Scientifique ^0 Info/Liv_In_Paris/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229083A9-99E6-40DF-8AA5-5EE58F71C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F03D0E2-DBAC-4352-A19F-D385E2D7B1BF}"/>
+    <workbookView xWindow="9495" yWindow="0" windowWidth="9810" windowHeight="15585" activeTab="1" xr2:uid="{7F03D0E2-DBAC-4352-A19F-D385E2D7B1BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Noeuds" sheetId="1" r:id="rId1"/>
@@ -9179,8 +9179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9554A256-CB03-4F66-9F1C-0720CFC4CDC2}">
   <dimension ref="A1:E332"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D332" sqref="D332"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>